<commit_message>
Updates to HP assay recipe sheets
Designated "print area" on recipe sheets before printing
</commit_message>
<xml_diff>
--- a/Biochemistry/Hydroxyproline Assay/RecipeSheets/ChloramineT_soln_recipe.xlsx
+++ b/Biochemistry/Hydroxyproline Assay/RecipeSheets/ChloramineT_soln_recipe.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atya222\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atya222\Documents\GitHub\Protocols\Biochemistry\Hydroxyproline Assay\RecipeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648A5FB6-8BDC-4B41-86DD-2185D33592AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CE6E4F-49EC-4D9C-A34E-9491B08B2EE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="500mL" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'500mL'!$A$1:$J$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'500mL'!$A$1:$J$6</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
 </workbook>
@@ -401,23 +401,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -855,7 +855,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -873,10 +873,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="23"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -912,10 +912,10 @@
       <c r="G4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="20" t="s">
         <v>14</v>
       </c>
       <c r="J4" s="16" t="s">
@@ -943,19 +943,19 @@
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="21"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="21" t="s">
         <v>18</v>
       </c>
       <c r="J6" s="10"/>
@@ -1010,18 +1010,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1248,6 +1248,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C3833AD-3BAD-44F9-A428-5312EFC8FF4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33AFEA7C-ECB0-4A51-9E17-02E120CDEEE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -1260,14 +1268,6 @@
     <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
     <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C3833AD-3BAD-44F9-A428-5312EFC8FF4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>